<commit_message>
Update, work from the UI, choose the excel file, choose directory, start the process, call the google API, get the distance, create a pdf, and save it on directory. Tests are not terminated. Miss ProgressBar, Icon, Title app.
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
   <si>
     <t>Service</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH3"/>
+  <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,6 +842,254 @@
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T4" s="4">
+        <v>12</v>
+      </c>
+      <c r="U4" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="V4" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T5" s="4">
+        <v>12</v>
+      </c>
+      <c r="U5" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="V5" s="4">
+        <v>64.8</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="T6" s="4">
+        <v>1</v>
+      </c>
+      <c r="U6" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="V6" s="4">
+        <v>5.4</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>